<commit_message>
can pass one case
</commit_message>
<xml_diff>
--- a/data/test_user_data.xlsx
+++ b/data/test_user_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="11020" activeTab="1"/>
+    <workbookView windowWidth="25600" windowHeight="9300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestUserLogin" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>case_name</t>
   </si>
@@ -59,11 +59,14 @@
     <t>test_accountant_price</t>
   </si>
   <si>
-    <t>https://pf.senguo.cc/accountant/home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"action": "cashier_list","_xsrf": "2|a14c572a|467af26ecd63e941f2816fc1b959a89d|1560909123"}
+    <t>https://pf.senguo.cc/boss/goods/stock/allot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"action": "get_storage_allocate_nofify_info","_xsrf": "2|ee1afba2|092c5ee6823545c9bdd7c349f60f0415|1560909123"}
 </t>
+  </si>
+  <si>
+    <t>{"success": true, "notify_dict": {"allocate_out_num": 0, "allocate_in_num": 0, "if_notify": 0}}</t>
   </si>
   <si>
     <t>test_user_reg_exist</t>
@@ -87,9 +90,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -129,6 +132,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -143,26 +160,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -174,6 +184,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -181,28 +229,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -213,57 +264,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,6 +287,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -296,13 +323,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,144 +456,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,45 +480,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -569,153 +533,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -753,8 +756,8 @@
   </cellXfs>
   <cellStyles count="53">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_" xfId="1"/>
-    <cellStyle name="常规 2" xfId="2"/>
+    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_" xfId="2"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="3" builtinId="52"/>
     <cellStyle name="20% - 强调文字颜色 4" xfId="4" builtinId="42"/>
     <cellStyle name="强调文字颜色 4" xfId="5" builtinId="41"/>
@@ -1180,7 +1183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="63" spans="1:5">
+    <row r="2" s="2" customFormat="1" ht="94" spans="1:5">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -1193,14 +1196,16 @@
       <c r="D2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="125" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>7</v>
@@ -1209,12 +1214,12 @@
         <v>8</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://pf.senguo.cc/accountant/home" tooltip="https://pf.senguo.cc/accountant/home"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://pf.senguo.cc/boss/goods/stock/allot" tooltip="https://pf.senguo.cc/boss/goods/stock/allot"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>